<commit_message>
Fill out form for ModelWorkbench
</commit_message>
<xml_diff>
--- a/doc/ModelingWorkbench_FeatureConfiguration.xlsx
+++ b/doc/ModelingWorkbench_FeatureConfiguration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Judith Michael\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\digitalgardeners\repo\mps-lwc25\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3358ED40-FEE8-4E3E-9FED-070D3D5343D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D18146-D3E4-4C64-A906-E2D976C130A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9765" yWindow="1305" windowWidth="16845" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="121">
   <si>
     <t>Feature</t>
   </si>
@@ -268,6 +268,126 @@
   </si>
   <si>
     <t>│   │   │   │   └── Specialization</t>
+  </si>
+  <si>
+    <t>limited support</t>
+  </si>
+  <si>
+    <t>Math notation available from community extensions</t>
+  </si>
+  <si>
+    <t>Additional usability and language maintainability through grammar cells and mixed notations via richtext (both via community extensions)</t>
+  </si>
+  <si>
+    <t>Diagrammatic notation from community extensions, custom cells (e.g. pictures, any java-based UI element) possible</t>
+  </si>
+  <si>
+    <t>Tabular notation from community extensions for advanced (e.g. sparse) tables, grid layout for simple tables</t>
+  </si>
+  <si>
+    <t>Tree notation from community extensions</t>
+  </si>
+  <si>
+    <t>Through cell-granular editors and their styling</t>
+  </si>
+  <si>
+    <t>Any java libraries supporting fluent API have automatic import and generation of baseLanguage stubs</t>
+  </si>
+  <si>
+    <t>baseLanguage can be mixed with other metalanguages (e.g. with smodel query language)</t>
+  </si>
+  <si>
+    <t>Extension and embedding of baseLanguage in a DSL possible</t>
+  </si>
+  <si>
+    <t>All metalanguages (editors, structure, generator, typesystem, ...) are external; nearly all of them are extensible</t>
+  </si>
+  <si>
+    <t>Via textgen aspect or plaintextgen language</t>
+  </si>
+  <si>
+    <t>Modular, extensible, and incremental template-based generation via default generator mechanism, function-based generation via shadowmodels, Dclare4MPS, and translator framework (to be opensourced as part of ALEF)</t>
+  </si>
+  <si>
+    <t>Via community-provided interpreter aspect</t>
+  </si>
+  <si>
+    <t>Only in certain contexts, e.g. string literals and richtext</t>
+  </si>
+  <si>
+    <t>Any kind of extra information (e.g. layout for a diagram) can be stored transparently in the form of node attributes</t>
+  </si>
+  <si>
+    <t>A big strength of MPS</t>
+  </si>
+  <si>
+    <t>Generic node-based diff, using editor aspect (concrete syntax definition)</t>
+  </si>
+  <si>
+    <t>By default proper node id-based references, but name (re)binding possible with resolveinfo</t>
+  </si>
+  <si>
+    <t>Transient models and tracing (backward as well as forward) of nodes in different generation steps and to their corresponding transformation rules</t>
+  </si>
+  <si>
+    <t>Through shadowmodels, Dclare4MPS or translator framework</t>
+  </si>
+  <si>
+    <t>Notable examples: full java debugging in baseLanguage, full C debugging in mbeddr, computation tree debugger in KernelF</t>
+  </si>
+  <si>
+    <t>More generic than just calls: references (which may model calls) are visualized and there editing helps</t>
+  </si>
+  <si>
+    <t>Basic view is the Node Explorer; more convenient view is the reflective editor</t>
+  </si>
+  <si>
+    <t>Possible via editor hints and simplified for end users through Projection menu</t>
+  </si>
+  <si>
+    <t>In addition, (cell-granular) mixing of different notations in a model possible</t>
+  </si>
+  <si>
+    <t>Not an issue due to UUID-based node identification, but name-based (re)binding checked against concept instance types possible</t>
+  </si>
+  <si>
+    <t>Solver-based typesystem unification, including debugging support</t>
+  </si>
+  <si>
+    <t>MPS does not intertwine semantics directly into the language grammar, but there is no fundamental limtation to generate to a proving system like Coq; however we are not aware of any effort in that direction for MPS-based languages</t>
+  </si>
+  <si>
+    <t>Several pre-input and post-input checks available in the form of structure definition and some constraints</t>
+  </si>
+  <si>
+    <t>Not out of the box available (as there was never seen a need), but it is easy enough to make this generically supported</t>
+  </si>
+  <si>
+    <t>While there is no out-of-the-box omniscient debugger, the debugging framework allows creating one for a language</t>
+  </si>
+  <si>
+    <t>Typical pattern is to have a test language on the same abstraction level as the language you want to test</t>
+  </si>
+  <si>
+    <t>Operational transform-based CRDT possible via Modelix plugin in combination with Modelix repository</t>
+  </si>
+  <si>
+    <t>MPS-to-MPS serverless model synchronization possible via Dclare4MPS</t>
+  </si>
+  <si>
+    <t>CRDT-based collaboration MPS-to-MPS or MPS-to-other clients</t>
+  </si>
+  <si>
+    <t>Connection to git out of the box, others possible via plugins</t>
+  </si>
+  <si>
+    <t>Java-based desktop app</t>
+  </si>
+  <si>
+    <t>Backend: fully containerized MPS for model storage and model checking services possible; Front-end: manual web-based editor definition using Modelix API possible and limited text-based automatic web-based editor derivation from MPS language definition possible</t>
+  </si>
+  <si>
+    <t>All of MPS functionality is the OpenAPI set of libraries with the metalanguages as external DSLs to abstract those APIs</t>
   </si>
 </sst>
 </file>
@@ -378,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -386,19 +506,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -431,12 +562,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83EE3E99-DC55-4AA5-9373-CE7CD4B397EB}" name="Tableau2" displayName="Tableau2" ref="A1:C73" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83EE3E99-DC55-4AA5-9373-CE7CD4B397EB}" name="Tableau2" displayName="Tableau2" ref="A1:C73" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:C73" xr:uid="{83EE3E99-DC55-4AA5-9373-CE7CD4B397EB}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{7079AA7E-1D06-47FE-BBEE-8677B9F81300}" name="Feature" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{2525B41F-5756-4483-BC59-2CE0C7805AB6}" name="&lt;Language workbench name&gt;"/>
-    <tableColumn id="3" xr3:uid="{2B497C5B-379C-4E34-A53A-0CC17C1E85C7}" name="Comments"/>
+    <tableColumn id="1" xr3:uid="{7079AA7E-1D06-47FE-BBEE-8677B9F81300}" name="Feature" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{2525B41F-5756-4483-BC59-2CE0C7805AB6}" name="&lt;Language workbench name&gt;" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{2B497C5B-379C-4E34-A53A-0CC17C1E85C7}" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -708,10 +839,10 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43" customWidth="1"/>
     <col min="2" max="2" width="31.140625" customWidth="1"/>
@@ -735,10 +866,10 @@
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -746,10 +877,10 @@
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -757,64 +888,90 @@
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="B5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="E7" s="5" t="s">
+      <c r="B7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
+      <c r="B8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="E9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="8"/>
+      <c r="B9" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="E10" s="7" t="s">
+      <c r="B10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="E10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -822,25 +979,25 @@
       <c r="A11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="9" t="s">
+      <c r="B11" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="10"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="3"/>
@@ -850,8 +1007,12 @@
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="B13" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>88</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
@@ -859,8 +1020,12 @@
       <c r="A14" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>89</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
@@ -868,8 +1033,12 @@
       <c r="A15" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
@@ -877,19 +1046,23 @@
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="E16" s="4"/>
+      <c r="B16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B17" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -897,10 +1070,10 @@
       <c r="A18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -908,31 +1081,43 @@
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="B19" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="B21" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="B22" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -940,10 +1125,10 @@
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="B23" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -951,31 +1136,43 @@
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="B24" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="B25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="B26" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="B27" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -983,52 +1180,66 @@
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="B28" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="10"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="B29" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="10"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="B30" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="10"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="B31" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="10"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="B32" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="B33" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="10"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="B34" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1036,59 +1247,79 @@
       <c r="A35" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="B35" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="B36" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="10"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="B37" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="10"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+      <c r="B38" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="10"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="B39" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="10"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
+      <c r="B40" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+      <c r="B41" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="2" t="s">
+      <c r="B42" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1096,31 +1327,43 @@
       <c r="A43" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="B43" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
+      <c r="B44" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="B45" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="2" t="s">
+      <c r="B46" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1128,24 +1371,32 @@
       <c r="A47" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
+      <c r="B47" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+      <c r="B48" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="B49" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1153,52 +1404,74 @@
       <c r="A50" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+      <c r="B50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="B51" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="B52" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
+      <c r="B53" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
+      <c r="B54" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="10"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
+      <c r="B55" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C56" s="2" t="s">
+      <c r="B56" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1206,31 +1479,43 @@
       <c r="A57" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+      <c r="B57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="B58" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+      <c r="B59" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60" s="2" t="s">
+      <c r="B60" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1238,10 +1523,10 @@
       <c r="A61" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C61" s="2" t="s">
+      <c r="B61" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1249,10 +1534,10 @@
       <c r="A62" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62" s="2" t="s">
+      <c r="B62" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1260,24 +1545,29 @@
       <c r="A63" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
+      <c r="B63" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C65" s="2" t="s">
+      <c r="B65" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1285,31 +1575,43 @@
       <c r="A66" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
+      <c r="B66" t="s">
+        <v>81</v>
+      </c>
+      <c r="C66" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
+      <c r="B67" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
+      <c r="B68" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C69" s="2" t="s">
+      <c r="B69" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1317,10 +1619,10 @@
       <c r="A70" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C70" s="2" t="s">
+      <c r="B70" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1328,22 +1630,34 @@
       <c r="A71" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
+      <c r="B71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
+      <c r="B72" t="s">
+        <v>81</v>
+      </c>
+      <c r="C72" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>

</xml_diff>